<commit_message>
corrected values from ecc
</commit_message>
<xml_diff>
--- a/data/ecc_supply_to_mcc.xlsx
+++ b/data/ecc_supply_to_mcc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschu\Documents\github\MaterialExergyPaper2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F11EC2-08A2-4A49-A147-A8BF7F012348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90538A6-1E62-4C57-A239-065037FBAE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,17 +507,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -526,6 +519,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="63" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193:F212"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="63" workbookViewId="0">
+      <selection activeCell="J205" sqref="J205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6093,48 +6093,48 @@
       <c r="B42" s="7">
         <v>1</v>
       </c>
-      <c r="AS42" s="8" t="s">
+      <c r="AS42" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="AT42" s="9"/>
-      <c r="AU42" s="9"/>
-      <c r="AV42" s="9"/>
-      <c r="AW42" s="9"/>
-      <c r="AX42" s="9"/>
-      <c r="AY42" s="9"/>
-      <c r="AZ42" s="9"/>
-      <c r="BA42" s="9"/>
-      <c r="BB42" s="9"/>
-      <c r="BC42" s="9"/>
-      <c r="BD42" s="9"/>
-      <c r="BE42" s="9"/>
-      <c r="BF42" s="9"/>
-      <c r="BG42" s="9"/>
-      <c r="BH42" s="9"/>
-      <c r="BI42" s="9"/>
-      <c r="BJ42" s="9"/>
-      <c r="BK42" s="9"/>
-      <c r="BO42" s="8" t="s">
+      <c r="AT42" s="14"/>
+      <c r="AU42" s="14"/>
+      <c r="AV42" s="14"/>
+      <c r="AW42" s="14"/>
+      <c r="AX42" s="14"/>
+      <c r="AY42" s="14"/>
+      <c r="AZ42" s="14"/>
+      <c r="BA42" s="14"/>
+      <c r="BB42" s="14"/>
+      <c r="BC42" s="14"/>
+      <c r="BD42" s="14"/>
+      <c r="BE42" s="14"/>
+      <c r="BF42" s="14"/>
+      <c r="BG42" s="14"/>
+      <c r="BH42" s="14"/>
+      <c r="BI42" s="14"/>
+      <c r="BJ42" s="14"/>
+      <c r="BK42" s="14"/>
+      <c r="BO42" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="BP42" s="9"/>
-      <c r="BQ42" s="9"/>
-      <c r="BR42" s="9"/>
-      <c r="BS42" s="9"/>
-      <c r="BT42" s="9"/>
-      <c r="BU42" s="9"/>
-      <c r="BV42" s="9"/>
-      <c r="BW42" s="9"/>
-      <c r="BX42" s="9"/>
-      <c r="BY42" s="9"/>
-      <c r="BZ42" s="9"/>
-      <c r="CA42" s="9"/>
-      <c r="CB42" s="9"/>
-      <c r="CC42" s="9"/>
-      <c r="CD42" s="9"/>
-      <c r="CE42" s="9"/>
-      <c r="CF42" s="9"/>
-      <c r="CG42" s="9"/>
+      <c r="BP42" s="14"/>
+      <c r="BQ42" s="14"/>
+      <c r="BR42" s="14"/>
+      <c r="BS42" s="14"/>
+      <c r="BT42" s="14"/>
+      <c r="BU42" s="14"/>
+      <c r="BV42" s="14"/>
+      <c r="BW42" s="14"/>
+      <c r="BX42" s="14"/>
+      <c r="BY42" s="14"/>
+      <c r="BZ42" s="14"/>
+      <c r="CA42" s="14"/>
+      <c r="CB42" s="14"/>
+      <c r="CC42" s="14"/>
+      <c r="CD42" s="14"/>
+      <c r="CE42" s="14"/>
+      <c r="CF42" s="14"/>
+      <c r="CG42" s="14"/>
     </row>
     <row r="43" spans="1:85">
       <c r="A43" s="2" t="s">
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="46" spans="1:85">
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="13" t="s">
         <v>99</v>
       </c>
       <c r="AR46" s="2" t="s">
@@ -8701,27 +8701,27 @@
       </c>
     </row>
     <row r="86" spans="44:67">
-      <c r="AS86" s="8" t="s">
+      <c r="AS86" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="AT86" s="9"/>
-      <c r="AU86" s="9"/>
-      <c r="AV86" s="9"/>
-      <c r="AW86" s="9"/>
-      <c r="AX86" s="9"/>
-      <c r="AY86" s="9"/>
-      <c r="AZ86" s="9"/>
-      <c r="BA86" s="9"/>
-      <c r="BB86" s="9"/>
-      <c r="BC86" s="9"/>
-      <c r="BD86" s="9"/>
-      <c r="BE86" s="9"/>
-      <c r="BF86" s="9"/>
-      <c r="BG86" s="9"/>
-      <c r="BH86" s="9"/>
-      <c r="BI86" s="9"/>
-      <c r="BJ86" s="9"/>
-      <c r="BK86" s="9"/>
+      <c r="AT86" s="14"/>
+      <c r="AU86" s="14"/>
+      <c r="AV86" s="14"/>
+      <c r="AW86" s="14"/>
+      <c r="AX86" s="14"/>
+      <c r="AY86" s="14"/>
+      <c r="AZ86" s="14"/>
+      <c r="BA86" s="14"/>
+      <c r="BB86" s="14"/>
+      <c r="BC86" s="14"/>
+      <c r="BD86" s="14"/>
+      <c r="BE86" s="14"/>
+      <c r="BF86" s="14"/>
+      <c r="BG86" s="14"/>
+      <c r="BH86" s="14"/>
+      <c r="BI86" s="14"/>
+      <c r="BJ86" s="14"/>
+      <c r="BK86" s="14"/>
     </row>
     <row r="89" spans="44:67" ht="181.8">
       <c r="AS89" s="3" t="s">
@@ -11506,28 +11506,28 @@
       </c>
     </row>
     <row r="130" spans="1:67">
-      <c r="AS130" s="8" t="s">
+      <c r="AS130" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="AT130" s="9"/>
-      <c r="AU130" s="9"/>
-      <c r="AV130" s="9"/>
-      <c r="AW130" s="9"/>
-      <c r="AX130" s="9"/>
-      <c r="AY130" s="9"/>
-      <c r="AZ130" s="9"/>
-      <c r="BA130" s="9"/>
-      <c r="BB130" s="9"/>
-      <c r="BC130" s="9"/>
-      <c r="BD130" s="9"/>
-      <c r="BE130" s="9"/>
-      <c r="BF130" s="9"/>
-      <c r="BG130" s="9"/>
-      <c r="BH130" s="9"/>
-      <c r="BI130" s="9"/>
-      <c r="BJ130" s="9"/>
-      <c r="BK130" s="9"/>
-      <c r="BO130" s="8" t="s">
+      <c r="AT130" s="14"/>
+      <c r="AU130" s="14"/>
+      <c r="AV130" s="14"/>
+      <c r="AW130" s="14"/>
+      <c r="AX130" s="14"/>
+      <c r="AY130" s="14"/>
+      <c r="AZ130" s="14"/>
+      <c r="BA130" s="14"/>
+      <c r="BB130" s="14"/>
+      <c r="BC130" s="14"/>
+      <c r="BD130" s="14"/>
+      <c r="BE130" s="14"/>
+      <c r="BF130" s="14"/>
+      <c r="BG130" s="14"/>
+      <c r="BH130" s="14"/>
+      <c r="BI130" s="14"/>
+      <c r="BJ130" s="14"/>
+      <c r="BK130" s="14"/>
+      <c r="BO130" s="13" t="s">
         <v>90</v>
       </c>
     </row>
@@ -14029,48 +14029,48 @@
       </c>
     </row>
     <row r="153" spans="1:41">
-      <c r="B153" s="8" t="s">
+      <c r="B153" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C153" s="9"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="9"/>
-      <c r="F153" s="9"/>
-      <c r="G153" s="9"/>
-      <c r="H153" s="9"/>
-      <c r="I153" s="9"/>
-      <c r="J153" s="9"/>
-      <c r="K153" s="9"/>
-      <c r="L153" s="9"/>
-      <c r="M153" s="9"/>
-      <c r="N153" s="9"/>
-      <c r="O153" s="9"/>
-      <c r="P153" s="9"/>
-      <c r="Q153" s="9"/>
-      <c r="R153" s="9"/>
-      <c r="S153" s="9"/>
-      <c r="T153" s="9"/>
-      <c r="U153" s="9"/>
-      <c r="V153" s="9"/>
-      <c r="W153" s="9"/>
-      <c r="X153" s="9"/>
-      <c r="Y153" s="9"/>
-      <c r="Z153" s="9"/>
-      <c r="AA153" s="9"/>
-      <c r="AB153" s="9"/>
-      <c r="AC153" s="9"/>
-      <c r="AD153" s="9"/>
-      <c r="AE153" s="9"/>
-      <c r="AF153" s="9"/>
-      <c r="AG153" s="9"/>
-      <c r="AH153" s="9"/>
-      <c r="AI153" s="9"/>
-      <c r="AJ153" s="9"/>
-      <c r="AK153" s="9"/>
-      <c r="AL153" s="9"/>
-      <c r="AM153" s="9"/>
-      <c r="AN153" s="9"/>
-      <c r="AO153" s="9"/>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="14"/>
+      <c r="I153" s="14"/>
+      <c r="J153" s="14"/>
+      <c r="K153" s="14"/>
+      <c r="L153" s="14"/>
+      <c r="M153" s="14"/>
+      <c r="N153" s="14"/>
+      <c r="O153" s="14"/>
+      <c r="P153" s="14"/>
+      <c r="Q153" s="14"/>
+      <c r="R153" s="14"/>
+      <c r="S153" s="14"/>
+      <c r="T153" s="14"/>
+      <c r="U153" s="14"/>
+      <c r="V153" s="14"/>
+      <c r="W153" s="14"/>
+      <c r="X153" s="14"/>
+      <c r="Y153" s="14"/>
+      <c r="Z153" s="14"/>
+      <c r="AA153" s="14"/>
+      <c r="AB153" s="14"/>
+      <c r="AC153" s="14"/>
+      <c r="AD153" s="14"/>
+      <c r="AE153" s="14"/>
+      <c r="AF153" s="14"/>
+      <c r="AG153" s="14"/>
+      <c r="AH153" s="14"/>
+      <c r="AI153" s="14"/>
+      <c r="AJ153" s="14"/>
+      <c r="AK153" s="14"/>
+      <c r="AL153" s="14"/>
+      <c r="AM153" s="14"/>
+      <c r="AN153" s="14"/>
+      <c r="AO153" s="14"/>
     </row>
     <row r="156" spans="1:41" ht="184.8">
       <c r="B156" s="3" t="s">
@@ -17570,48 +17570,48 @@
       </c>
     </row>
     <row r="184" spans="1:41">
-      <c r="B184" s="8" t="s">
+      <c r="B184" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C184" s="9"/>
-      <c r="D184" s="9"/>
-      <c r="E184" s="9"/>
-      <c r="F184" s="9"/>
-      <c r="G184" s="9"/>
-      <c r="H184" s="9"/>
-      <c r="I184" s="9"/>
-      <c r="J184" s="9"/>
-      <c r="K184" s="9"/>
-      <c r="L184" s="9"/>
-      <c r="M184" s="9"/>
-      <c r="N184" s="9"/>
-      <c r="O184" s="9"/>
-      <c r="P184" s="9"/>
-      <c r="Q184" s="9"/>
-      <c r="R184" s="9"/>
-      <c r="S184" s="9"/>
-      <c r="T184" s="9"/>
-      <c r="U184" s="9"/>
-      <c r="V184" s="9"/>
-      <c r="W184" s="9"/>
-      <c r="X184" s="9"/>
-      <c r="Y184" s="9"/>
-      <c r="Z184" s="9"/>
-      <c r="AA184" s="9"/>
-      <c r="AB184" s="9"/>
-      <c r="AC184" s="9"/>
-      <c r="AD184" s="9"/>
-      <c r="AE184" s="9"/>
-      <c r="AF184" s="9"/>
-      <c r="AG184" s="9"/>
-      <c r="AH184" s="9"/>
-      <c r="AI184" s="9"/>
-      <c r="AJ184" s="9"/>
-      <c r="AK184" s="9"/>
-      <c r="AL184" s="9"/>
-      <c r="AM184" s="9"/>
-      <c r="AN184" s="9"/>
-      <c r="AO184" s="9"/>
+      <c r="C184" s="14"/>
+      <c r="D184" s="14"/>
+      <c r="E184" s="14"/>
+      <c r="F184" s="14"/>
+      <c r="G184" s="14"/>
+      <c r="H184" s="14"/>
+      <c r="I184" s="14"/>
+      <c r="J184" s="14"/>
+      <c r="K184" s="14"/>
+      <c r="L184" s="14"/>
+      <c r="M184" s="14"/>
+      <c r="N184" s="14"/>
+      <c r="O184" s="14"/>
+      <c r="P184" s="14"/>
+      <c r="Q184" s="14"/>
+      <c r="R184" s="14"/>
+      <c r="S184" s="14"/>
+      <c r="T184" s="14"/>
+      <c r="U184" s="14"/>
+      <c r="V184" s="14"/>
+      <c r="W184" s="14"/>
+      <c r="X184" s="14"/>
+      <c r="Y184" s="14"/>
+      <c r="Z184" s="14"/>
+      <c r="AA184" s="14"/>
+      <c r="AB184" s="14"/>
+      <c r="AC184" s="14"/>
+      <c r="AD184" s="14"/>
+      <c r="AE184" s="14"/>
+      <c r="AF184" s="14"/>
+      <c r="AG184" s="14"/>
+      <c r="AH184" s="14"/>
+      <c r="AI184" s="14"/>
+      <c r="AJ184" s="14"/>
+      <c r="AK184" s="14"/>
+      <c r="AL184" s="14"/>
+      <c r="AM184" s="14"/>
+      <c r="AN184" s="14"/>
+      <c r="AO184" s="14"/>
     </row>
     <row r="190" spans="1:41">
       <c r="B190" s="12" t="s">
@@ -17628,15 +17628,15 @@
       <c r="A193" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B193" s="13">
+      <c r="B193" s="10">
         <f>SUM(AS90:AS129)</f>
         <v>2.7035257213616101E-11</v>
       </c>
-      <c r="D193" s="13">
+      <c r="D193" s="10">
         <f>SUM(B134:AO134)</f>
         <v>1.0711098672120199E-11</v>
       </c>
-      <c r="F193" s="13">
+      <c r="F193" s="10">
         <f>B193-D193</f>
         <v>1.6324158541495901E-11</v>
       </c>
@@ -17645,209 +17645,209 @@
       <c r="A194" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B194" s="13">
-        <f t="shared" ref="B194:B211" si="0">SUM(AS91:AS130)</f>
-        <v>2.7035257213616101E-11</v>
-      </c>
-      <c r="D194" s="13">
-        <f t="shared" ref="D194:D211" si="1">SUM(B135:AO135)</f>
+      <c r="B194" s="10">
+        <f>SUM(AT90:AT129)</f>
+        <v>-3.93451133810275E-13</v>
+      </c>
+      <c r="D194" s="10">
+        <f>SUM(B135:AO135)</f>
         <v>-5.6964684791701695E-14</v>
       </c>
-      <c r="F194" s="13">
-        <f t="shared" ref="F194:F211" si="2">B194-D194</f>
-        <v>2.7092221898407803E-11</v>
+      <c r="F194" s="10">
+        <f t="shared" ref="F194:F211" si="0">B194-D194</f>
+        <v>-3.3648644901857331E-13</v>
       </c>
     </row>
     <row r="195" spans="1:6">
       <c r="A195" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B195" s="13">
+      <c r="B195" s="10">
+        <f>SUM(AU90:AU129)</f>
+        <v>80113.817233021196</v>
+      </c>
+      <c r="D195" s="10">
+        <f t="shared" ref="D194:D211" si="1">SUM(B136:AO136)</f>
+        <v>16030.243919636299</v>
+      </c>
+      <c r="F195" s="10">
         <f t="shared" si="0"/>
-        <v>2.7035257213616101E-11</v>
-      </c>
-      <c r="D195" s="13">
-        <f t="shared" si="1"/>
-        <v>16030.243919636299</v>
-      </c>
-      <c r="F195" s="13">
-        <f t="shared" si="2"/>
-        <v>-16030.243919636272</v>
+        <v>64083.573313384899</v>
       </c>
     </row>
     <row r="196" spans="1:6">
       <c r="A196" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B196" s="13">
-        <f t="shared" si="0"/>
-        <v>2.7035257213616101E-11</v>
-      </c>
-      <c r="D196" s="13">
+      <c r="B196" s="10">
+        <f>SUM(AV90:AV129)</f>
+        <v>3207824.8619437884</v>
+      </c>
+      <c r="D196" s="10">
         <f t="shared" si="1"/>
         <v>3202004.12978845</v>
       </c>
-      <c r="F196" s="13">
-        <f t="shared" si="2"/>
-        <v>-3202004.12978845</v>
+      <c r="F196" s="10">
+        <f t="shared" si="0"/>
+        <v>5820.7321553383954</v>
       </c>
     </row>
     <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B197" s="13">
-        <f t="shared" si="0"/>
-        <v>2.7035257213616101E-11</v>
-      </c>
-      <c r="D197" s="13">
+      <c r="B197" s="10">
+        <f>SUM(AW90:AW129)</f>
+        <v>3.9089210146248001E-11</v>
+      </c>
+      <c r="D197" s="10">
         <f t="shared" si="1"/>
         <v>2.7035253348937101E-11</v>
       </c>
-      <c r="F197" s="13">
-        <f t="shared" si="2"/>
-        <v>3.8646789991232337E-18</v>
+      <c r="F197" s="10">
+        <f t="shared" si="0"/>
+        <v>1.20539567973109E-11</v>
       </c>
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="13">
-        <f t="shared" si="0"/>
-        <v>2.7035257213616101E-11</v>
-      </c>
-      <c r="D198" s="13">
+      <c r="B198" s="10">
+        <f>SUM(AX90:AX129)</f>
+        <v>-8.2794817109293496E-10</v>
+      </c>
+      <c r="D198" s="10">
         <f t="shared" si="1"/>
         <v>-2.1850384186490701E-10</v>
       </c>
-      <c r="F198" s="13">
-        <f t="shared" si="2"/>
-        <v>2.4553909907852311E-10</v>
+      <c r="F198" s="10">
+        <f t="shared" si="0"/>
+        <v>-6.0944432922802798E-10</v>
       </c>
     </row>
     <row r="199" spans="1:6">
       <c r="A199" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D199" s="13">
+      <c r="B199" s="10">
+        <f>SUM(AY90:AY129)</f>
+        <v>10407.5335702297</v>
+      </c>
+      <c r="D199" s="10">
         <f t="shared" si="1"/>
         <v>5653.4469866310001</v>
       </c>
-      <c r="F199" s="13">
-        <f t="shared" si="2"/>
-        <v>-5653.4469866310001</v>
+      <c r="F199" s="10">
+        <f t="shared" si="0"/>
+        <v>4754.0865835986997</v>
       </c>
     </row>
     <row r="200" spans="1:6">
       <c r="A200" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B200" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D200" s="13">
+      <c r="B200" s="10">
+        <f>SUM(AZ90:AZ129)</f>
+        <v>3284366.0335815852</v>
+      </c>
+      <c r="D200" s="10">
         <f t="shared" si="1"/>
         <v>1032997.83916021</v>
       </c>
-      <c r="F200" s="13">
-        <f t="shared" si="2"/>
-        <v>-1032997.83916021</v>
+      <c r="F200" s="10">
+        <f t="shared" si="0"/>
+        <v>2251368.1944213752</v>
       </c>
     </row>
     <row r="201" spans="1:6">
       <c r="A201" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B201" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B201" s="10">
+        <f>SUM(BA90:BA129)</f>
+        <v>4830.4442158522497</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D201" s="13">
+      <c r="D201" s="10">
         <f t="shared" si="1"/>
         <v>4830.4442158522497</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F201" s="13">
-        <f t="shared" si="2"/>
-        <v>-4830.4442158522497</v>
+      <c r="F201" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:6">
       <c r="A202" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B202" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D202" s="13">
+      <c r="B202" s="10">
+        <f>SUM(BB90:BB129)</f>
+        <v>184686.52821315001</v>
+      </c>
+      <c r="D202" s="10">
         <f t="shared" si="1"/>
         <v>184686.52821315001</v>
       </c>
-      <c r="F202" s="13">
-        <f t="shared" si="2"/>
-        <v>-184686.52821315001</v>
+      <c r="F202" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:6">
       <c r="A203" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B203" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D203" s="13">
+      <c r="B203" s="10">
+        <f>SUM(BC90:BC129)</f>
+        <v>5023.7890204089899</v>
+      </c>
+      <c r="D203" s="10">
         <f t="shared" si="1"/>
         <v>5023.7890204089899</v>
       </c>
-      <c r="F203" s="13">
-        <f t="shared" si="2"/>
-        <v>-5023.7890204089899</v>
+      <c r="F203" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B204" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D204" s="13">
+      <c r="B204" s="10">
+        <f>SUM(BD90:BD129)</f>
+        <v>82.091627997489695</v>
+      </c>
+      <c r="D204" s="10">
         <f t="shared" si="1"/>
         <v>82.091627997489695</v>
       </c>
-      <c r="F204" s="13">
-        <f t="shared" si="2"/>
-        <v>-82.091627997489695</v>
+      <c r="F204" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B205" s="13">
+      <c r="B205" s="10">
+        <f>SUM(BE90:BE129)</f>
+        <v>0</v>
+      </c>
+      <c r="D205" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F205" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D205" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F205" s="13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -17855,127 +17855,127 @@
       <c r="A206" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B206" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D206" s="13">
+      <c r="B206" s="10">
+        <f>SUM(BF90:BF129)</f>
+        <v>43.206119998678503</v>
+      </c>
+      <c r="D206" s="10">
         <f t="shared" si="1"/>
         <v>43.206119998678503</v>
       </c>
-      <c r="F206" s="13">
-        <f t="shared" si="2"/>
-        <v>-43.206119998678503</v>
+      <c r="F206" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:6">
       <c r="A207" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B207" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D207" s="13">
+      <c r="B207" s="10">
+        <f>SUM(BG90:BG129)</f>
+        <v>3749358.3680556798</v>
+      </c>
+      <c r="D207" s="10">
         <f t="shared" si="1"/>
         <v>3749358.3680556798</v>
       </c>
-      <c r="F207" s="13">
-        <f t="shared" si="2"/>
-        <v>-3749358.3680556798</v>
+      <c r="F207" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B208" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D208" s="13">
+      <c r="B208" s="10">
+        <f>SUM(BH90:BH129)</f>
+        <v>184686.52821315001</v>
+      </c>
+      <c r="D208" s="10">
         <f t="shared" si="1"/>
         <v>60946.554310340602</v>
       </c>
-      <c r="F208" s="13">
-        <f t="shared" si="2"/>
-        <v>-60946.554310340602</v>
+      <c r="F208" s="10">
+        <f t="shared" si="0"/>
+        <v>123739.9739028094</v>
       </c>
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B209" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D209" s="13">
+      <c r="B209" s="10">
+        <f>SUM(BI90:BI129)</f>
+        <v>958.99457187396001</v>
+      </c>
+      <c r="D209" s="10">
         <f t="shared" si="1"/>
         <v>958.99457187396001</v>
       </c>
-      <c r="F209" s="13">
-        <f t="shared" si="2"/>
-        <v>-958.99457187396001</v>
+      <c r="F209" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B210" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D210" s="13">
+      <c r="B210" s="10">
+        <f>SUM(BJ90:BJ129)</f>
+        <v>99968.352638963552</v>
+      </c>
+      <c r="D210" s="10">
         <f t="shared" si="1"/>
         <v>92166.861405407893</v>
       </c>
-      <c r="F210" s="13">
-        <f t="shared" si="2"/>
-        <v>-92166.861405407893</v>
+      <c r="F210" s="10">
+        <f t="shared" si="0"/>
+        <v>7801.4912335556583</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B211" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D211" s="13">
+      <c r="B211" s="10">
+        <f>SUM(BK90:BK129)</f>
+        <v>21683.690906267198</v>
+      </c>
+      <c r="D211" s="10">
         <f t="shared" si="1"/>
         <v>23208.442077419659</v>
       </c>
-      <c r="F211" s="13">
-        <f t="shared" si="2"/>
-        <v>-23208.442077419659</v>
+      <c r="F211" s="10">
+        <f t="shared" si="0"/>
+        <v>-1524.7511711524603</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="16.8">
-      <c r="B212" s="10" t="s">
+      <c r="B212" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C212" s="4"/>
-      <c r="D212" s="11" t="s">
+      <c r="D212" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F212" s="14" t="s">
+      <c r="F212" s="11" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="BO42:CG42"/>
+    <mergeCell ref="AS42:BK42"/>
+    <mergeCell ref="AS86:BK86"/>
+    <mergeCell ref="B46"/>
     <mergeCell ref="B190:H190"/>
     <mergeCell ref="B184:AO184"/>
     <mergeCell ref="AS130:BK130"/>
     <mergeCell ref="B153:AO153"/>
     <mergeCell ref="BO130"/>
-    <mergeCell ref="BO42:CG42"/>
-    <mergeCell ref="AS42:BK42"/>
-    <mergeCell ref="AS86:BK86"/>
-    <mergeCell ref="B46"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Q --> X for losses
</commit_message>
<xml_diff>
--- a/data/ecc_supply_to_mcc.xlsx
+++ b/data/ecc_supply_to_mcc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschu\Documents\github\MaterialExergyPaper2025\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90538A6-1E62-4C57-A239-065037FBAE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1A1B9-0A22-F54B-B3AD-93F4910C1E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38540" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZAF_2013_X" sheetId="1" r:id="rId1"/>
@@ -390,14 +390,14 @@
     <t>=</t>
   </si>
   <si>
-    <t>Q_loss</t>
+    <t>X_loss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -519,13 +519,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,30 +824,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="63" workbookViewId="0">
-      <selection activeCell="J205" sqref="J205"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="24" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="43" width="8.44140625"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="41" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="8.5"/>
     <col min="44" max="44" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="65" width="8.44140625"/>
+    <col min="45" max="65" width="8.5"/>
     <col min="66" max="66" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="181.8">
+    <row r="1" spans="1:85" ht="192" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>94</v>
       </c>
@@ -966,7 +974,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:85">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:85">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1222,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:85">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:85">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
@@ -1478,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:85">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:85">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1734,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:85">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1862,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:85">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1990,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:85">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2118,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:85">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2246,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:85">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2374,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:85">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2502,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:85">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2630,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:85">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -2758,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:85">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2886,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:85">
+    <row r="17" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3014,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:85">
+    <row r="18" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3142,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:85">
+    <row r="19" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -3270,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:85">
+    <row r="20" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -3398,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:85">
+    <row r="21" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -3526,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:85">
+    <row r="22" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -3654,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:85">
+    <row r="23" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3782,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:85">
+    <row r="24" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3910,7 +3918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:85">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -4038,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:85">
+    <row r="26" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -4166,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:85">
+    <row r="27" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -4294,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:85">
+    <row r="28" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -4422,7 +4430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:85">
+    <row r="29" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -4550,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:85">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -4678,7 +4686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:85">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -4806,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:85">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -4934,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:85">
+    <row r="33" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -5062,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:85">
+    <row r="34" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -5190,7 +5198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:85">
+    <row r="35" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>97</v>
       </c>
@@ -5318,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:85">
+    <row r="36" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
@@ -5446,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:85">
+    <row r="37" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -5574,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:85">
+    <row r="38" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
@@ -5702,7 +5710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:85">
+    <row r="39" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -5830,7 +5838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:85">
+    <row r="40" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -5958,7 +5966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:85">
+    <row r="41" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -6086,57 +6094,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:85">
+    <row r="42" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="7">
         <v>1</v>
       </c>
-      <c r="AS42" s="13" t="s">
+      <c r="AS42" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AT42" s="14"/>
-      <c r="AU42" s="14"/>
-      <c r="AV42" s="14"/>
-      <c r="AW42" s="14"/>
-      <c r="AX42" s="14"/>
-      <c r="AY42" s="14"/>
-      <c r="AZ42" s="14"/>
-      <c r="BA42" s="14"/>
-      <c r="BB42" s="14"/>
-      <c r="BC42" s="14"/>
-      <c r="BD42" s="14"/>
-      <c r="BE42" s="14"/>
-      <c r="BF42" s="14"/>
-      <c r="BG42" s="14"/>
-      <c r="BH42" s="14"/>
-      <c r="BI42" s="14"/>
-      <c r="BJ42" s="14"/>
-      <c r="BK42" s="14"/>
-      <c r="BO42" s="13" t="s">
+      <c r="AT42" s="13"/>
+      <c r="AU42" s="13"/>
+      <c r="AV42" s="13"/>
+      <c r="AW42" s="13"/>
+      <c r="AX42" s="13"/>
+      <c r="AY42" s="13"/>
+      <c r="AZ42" s="13"/>
+      <c r="BA42" s="13"/>
+      <c r="BB42" s="13"/>
+      <c r="BC42" s="13"/>
+      <c r="BD42" s="13"/>
+      <c r="BE42" s="13"/>
+      <c r="BF42" s="13"/>
+      <c r="BG42" s="13"/>
+      <c r="BH42" s="13"/>
+      <c r="BI42" s="13"/>
+      <c r="BJ42" s="13"/>
+      <c r="BK42" s="13"/>
+      <c r="BO42" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="BP42" s="14"/>
-      <c r="BQ42" s="14"/>
-      <c r="BR42" s="14"/>
-      <c r="BS42" s="14"/>
-      <c r="BT42" s="14"/>
-      <c r="BU42" s="14"/>
-      <c r="BV42" s="14"/>
-      <c r="BW42" s="14"/>
-      <c r="BX42" s="14"/>
-      <c r="BY42" s="14"/>
-      <c r="BZ42" s="14"/>
-      <c r="CA42" s="14"/>
-      <c r="CB42" s="14"/>
-      <c r="CC42" s="14"/>
-      <c r="CD42" s="14"/>
-      <c r="CE42" s="14"/>
-      <c r="CF42" s="14"/>
-      <c r="CG42" s="14"/>
-    </row>
-    <row r="43" spans="1:85">
+      <c r="BP42" s="13"/>
+      <c r="BQ42" s="13"/>
+      <c r="BR42" s="13"/>
+      <c r="BS42" s="13"/>
+      <c r="BT42" s="13"/>
+      <c r="BU42" s="13"/>
+      <c r="BV42" s="13"/>
+      <c r="BW42" s="13"/>
+      <c r="BX42" s="13"/>
+      <c r="BY42" s="13"/>
+      <c r="BZ42" s="13"/>
+      <c r="CA42" s="13"/>
+      <c r="CB42" s="13"/>
+      <c r="CC42" s="13"/>
+      <c r="CD42" s="13"/>
+      <c r="CE42" s="13"/>
+      <c r="CF42" s="13"/>
+      <c r="CG42" s="13"/>
+    </row>
+    <row r="43" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
@@ -6144,7 +6152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:85">
+    <row r="44" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
@@ -6152,7 +6160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:85" ht="181.8">
+    <row r="45" spans="1:85" ht="192" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
@@ -6217,8 +6225,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:85">
-      <c r="B46" s="13" t="s">
+    <row r="46" spans="1:85" x14ac:dyDescent="0.2">
+      <c r="B46" s="12" t="s">
         <v>99</v>
       </c>
       <c r="AR46" s="2" t="s">
@@ -6282,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:85">
+    <row r="47" spans="1:85" x14ac:dyDescent="0.2">
       <c r="AR47" s="2" t="s">
         <v>1</v>
       </c>
@@ -6344,7 +6352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:85">
+    <row r="48" spans="1:85" x14ac:dyDescent="0.2">
       <c r="AR48" s="2" t="s">
         <v>2</v>
       </c>
@@ -6406,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="44:63">
+    <row r="49" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR49" s="2" t="s">
         <v>3</v>
       </c>
@@ -6468,7 +6476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="44:63">
+    <row r="50" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR50" s="2" t="s">
         <v>4</v>
       </c>
@@ -6530,7 +6538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="44:63">
+    <row r="51" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR51" s="2" t="s">
         <v>5</v>
       </c>
@@ -6592,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="44:63">
+    <row r="52" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR52" s="2" t="s">
         <v>6</v>
       </c>
@@ -6654,7 +6662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="44:63">
+    <row r="53" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR53" s="2" t="s">
         <v>7</v>
       </c>
@@ -6716,7 +6724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="44:63">
+    <row r="54" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR54" s="2" t="s">
         <v>8</v>
       </c>
@@ -6778,7 +6786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="44:63">
+    <row r="55" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR55" s="2" t="s">
         <v>9</v>
       </c>
@@ -6840,7 +6848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="44:63">
+    <row r="56" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR56" s="2" t="s">
         <v>10</v>
       </c>
@@ -6902,7 +6910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="44:63">
+    <row r="57" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR57" s="2" t="s">
         <v>11</v>
       </c>
@@ -6964,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="44:63">
+    <row r="58" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR58" s="2" t="s">
         <v>12</v>
       </c>
@@ -7026,7 +7034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="44:63">
+    <row r="59" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR59" s="2" t="s">
         <v>13</v>
       </c>
@@ -7088,7 +7096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="44:63">
+    <row r="60" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR60" s="2" t="s">
         <v>14</v>
       </c>
@@ -7150,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="44:63">
+    <row r="61" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR61" s="2" t="s">
         <v>15</v>
       </c>
@@ -7212,7 +7220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="44:63">
+    <row r="62" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR62" s="2" t="s">
         <v>16</v>
       </c>
@@ -7274,7 +7282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="44:63">
+    <row r="63" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR63" s="2" t="s">
         <v>17</v>
       </c>
@@ -7336,7 +7344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="44:63">
+    <row r="64" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR64" s="2" t="s">
         <v>18</v>
       </c>
@@ -7398,7 +7406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="44:63">
+    <row r="65" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR65" s="2" t="s">
         <v>19</v>
       </c>
@@ -7460,7 +7468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="44:63">
+    <row r="66" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR66" s="2" t="s">
         <v>20</v>
       </c>
@@ -7522,7 +7530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="44:63">
+    <row r="67" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR67" s="2" t="s">
         <v>21</v>
       </c>
@@ -7584,7 +7592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="44:63">
+    <row r="68" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR68" s="2" t="s">
         <v>22</v>
       </c>
@@ -7646,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="44:63">
+    <row r="69" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR69" s="2" t="s">
         <v>23</v>
       </c>
@@ -7708,7 +7716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="44:63">
+    <row r="70" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR70" s="2" t="s">
         <v>24</v>
       </c>
@@ -7770,7 +7778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="44:63">
+    <row r="71" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR71" s="2" t="s">
         <v>25</v>
       </c>
@@ -7832,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="44:63">
+    <row r="72" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR72" s="2" t="s">
         <v>26</v>
       </c>
@@ -7894,7 +7902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="44:63">
+    <row r="73" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR73" s="2" t="s">
         <v>27</v>
       </c>
@@ -7956,7 +7964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="44:63">
+    <row r="74" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR74" s="2" t="s">
         <v>28</v>
       </c>
@@ -8018,7 +8026,7 @@
         <v>21683.690906267198</v>
       </c>
     </row>
-    <row r="75" spans="44:63">
+    <row r="75" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR75" s="2" t="s">
         <v>29</v>
       </c>
@@ -8080,7 +8088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="44:63">
+    <row r="76" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8142,7 +8150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="44:63">
+    <row r="77" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR77" s="2" t="s">
         <v>31</v>
       </c>
@@ -8204,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="44:63">
+    <row r="78" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR78" s="2" t="s">
         <v>32</v>
       </c>
@@ -8266,7 +8274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="44:63">
+    <row r="79" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR79" s="2" t="s">
         <v>33</v>
       </c>
@@ -8328,7 +8336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="44:63">
+    <row r="80" spans="44:63" x14ac:dyDescent="0.2">
       <c r="AR80" s="2" t="s">
         <v>34</v>
       </c>
@@ -8390,7 +8398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="44:67">
+    <row r="81" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR81" s="2" t="s">
         <v>35</v>
       </c>
@@ -8452,7 +8460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="44:67">
+    <row r="82" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR82" s="2" t="s">
         <v>36</v>
       </c>
@@ -8514,7 +8522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="44:67">
+    <row r="83" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR83" s="2" t="s">
         <v>37</v>
       </c>
@@ -8576,7 +8584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="44:67">
+    <row r="84" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR84" s="2" t="s">
         <v>38</v>
       </c>
@@ -8638,7 +8646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="44:67">
+    <row r="85" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR85" s="2" t="s">
         <v>39</v>
       </c>
@@ -8700,30 +8708,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="44:67">
-      <c r="AS86" s="13" t="s">
+    <row r="86" spans="44:67" x14ac:dyDescent="0.2">
+      <c r="AS86" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="AT86" s="14"/>
-      <c r="AU86" s="14"/>
-      <c r="AV86" s="14"/>
-      <c r="AW86" s="14"/>
-      <c r="AX86" s="14"/>
-      <c r="AY86" s="14"/>
-      <c r="AZ86" s="14"/>
-      <c r="BA86" s="14"/>
-      <c r="BB86" s="14"/>
-      <c r="BC86" s="14"/>
-      <c r="BD86" s="14"/>
-      <c r="BE86" s="14"/>
-      <c r="BF86" s="14"/>
-      <c r="BG86" s="14"/>
-      <c r="BH86" s="14"/>
-      <c r="BI86" s="14"/>
-      <c r="BJ86" s="14"/>
-      <c r="BK86" s="14"/>
-    </row>
-    <row r="89" spans="44:67" ht="181.8">
+      <c r="AT86" s="13"/>
+      <c r="AU86" s="13"/>
+      <c r="AV86" s="13"/>
+      <c r="AW86" s="13"/>
+      <c r="AX86" s="13"/>
+      <c r="AY86" s="13"/>
+      <c r="AZ86" s="13"/>
+      <c r="BA86" s="13"/>
+      <c r="BB86" s="13"/>
+      <c r="BC86" s="13"/>
+      <c r="BD86" s="13"/>
+      <c r="BE86" s="13"/>
+      <c r="BF86" s="13"/>
+      <c r="BG86" s="13"/>
+      <c r="BH86" s="13"/>
+      <c r="BI86" s="13"/>
+      <c r="BJ86" s="13"/>
+      <c r="BK86" s="13"/>
+    </row>
+    <row r="89" spans="44:67" ht="192" x14ac:dyDescent="0.2">
       <c r="AS89" s="3" t="s">
         <v>68</v>
       </c>
@@ -8785,7 +8793,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="44:67">
+    <row r="90" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR90" s="2" t="s">
         <v>0</v>
       </c>
@@ -8853,7 +8861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="44:67">
+    <row r="91" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR91" s="2" t="s">
         <v>1</v>
       </c>
@@ -8921,7 +8929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="44:67">
+    <row r="92" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR92" s="2" t="s">
         <v>2</v>
       </c>
@@ -8989,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="44:67">
+    <row r="93" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR93" s="2" t="s">
         <v>3</v>
       </c>
@@ -9057,7 +9065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="44:67">
+    <row r="94" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR94" s="2" t="s">
         <v>4</v>
       </c>
@@ -9125,7 +9133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="44:67">
+    <row r="95" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR95" s="2" t="s">
         <v>5</v>
       </c>
@@ -9193,7 +9201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="44:67">
+    <row r="96" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR96" s="2" t="s">
         <v>6</v>
       </c>
@@ -9261,7 +9269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="44:67">
+    <row r="97" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR97" s="2" t="s">
         <v>7</v>
       </c>
@@ -9329,7 +9337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="44:67">
+    <row r="98" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR98" s="2" t="s">
         <v>8</v>
       </c>
@@ -9397,7 +9405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="44:67">
+    <row r="99" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR99" s="2" t="s">
         <v>9</v>
       </c>
@@ -9465,7 +9473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="44:67">
+    <row r="100" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR100" s="2" t="s">
         <v>10</v>
       </c>
@@ -9533,7 +9541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="44:67">
+    <row r="101" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR101" s="2" t="s">
         <v>11</v>
       </c>
@@ -9601,7 +9609,7 @@
         <v>1058348.7350491199</v>
       </c>
     </row>
-    <row r="102" spans="44:67">
+    <row r="102" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR102" s="2" t="s">
         <v>12</v>
       </c>
@@ -9669,7 +9677,7 @@
         <v>29112.263489807599</v>
       </c>
     </row>
-    <row r="103" spans="44:67">
+    <row r="103" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR103" s="2" t="s">
         <v>13</v>
       </c>
@@ -9737,7 +9745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="44:67">
+    <row r="104" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR104" s="2" t="s">
         <v>14</v>
       </c>
@@ -9805,7 +9813,7 @@
         <v>117713.246391553</v>
       </c>
     </row>
-    <row r="105" spans="44:67">
+    <row r="105" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR105" s="2" t="s">
         <v>15</v>
       </c>
@@ -9873,7 +9881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="44:67">
+    <row r="106" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR106" s="2" t="s">
         <v>16</v>
       </c>
@@ -9941,7 +9949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="44:67">
+    <row r="107" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR107" s="2" t="s">
         <v>17</v>
       </c>
@@ -10009,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="44:67">
+    <row r="108" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR108" s="2" t="s">
         <v>18</v>
       </c>
@@ -10077,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="44:67">
+    <row r="109" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR109" s="2" t="s">
         <v>19</v>
       </c>
@@ -10145,7 +10153,7 @@
         <v>24.076233417548501</v>
       </c>
     </row>
-    <row r="110" spans="44:67">
+    <row r="110" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR110" s="2" t="s">
         <v>20</v>
       </c>
@@ -10213,7 +10221,7 @@
         <v>14864300.6683855</v>
       </c>
     </row>
-    <row r="111" spans="44:67">
+    <row r="111" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR111" s="2" t="s">
         <v>21</v>
       </c>
@@ -10281,7 +10289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="44:67">
+    <row r="112" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR112" s="2" t="s">
         <v>22</v>
       </c>
@@ -10349,7 +10357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="44:67">
+    <row r="113" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR113" s="2" t="s">
         <v>23</v>
       </c>
@@ -10417,7 +10425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="44:67">
+    <row r="114" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR114" s="2" t="s">
         <v>24</v>
       </c>
@@ -10485,7 +10493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="44:67">
+    <row r="115" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR115" s="2" t="s">
         <v>25</v>
       </c>
@@ -10553,7 +10561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="44:67">
+    <row r="116" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR116" s="2" t="s">
         <v>26</v>
       </c>
@@ -10621,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="44:67">
+    <row r="117" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR117" s="2" t="s">
         <v>27</v>
       </c>
@@ -10689,7 +10697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="44:67">
+    <row r="118" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR118" s="2" t="s">
         <v>28</v>
       </c>
@@ -10757,7 +10765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="44:67">
+    <row r="119" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR119" s="2" t="s">
         <v>29</v>
       </c>
@@ -10825,7 +10833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="44:67">
+    <row r="120" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR120" s="2" t="s">
         <v>30</v>
       </c>
@@ -10893,7 +10901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="44:67">
+    <row r="121" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR121" s="2" t="s">
         <v>31</v>
       </c>
@@ -10961,7 +10969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="44:67">
+    <row r="122" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR122" s="2" t="s">
         <v>32</v>
       </c>
@@ -11029,7 +11037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="44:67">
+    <row r="123" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR123" s="2" t="s">
         <v>33</v>
       </c>
@@ -11097,7 +11105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="44:67">
+    <row r="124" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR124" s="2" t="s">
         <v>34</v>
       </c>
@@ -11165,7 +11173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="44:67">
+    <row r="125" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR125" s="2" t="s">
         <v>35</v>
       </c>
@@ -11233,7 +11241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="44:67">
+    <row r="126" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR126" s="2" t="s">
         <v>36</v>
       </c>
@@ -11301,7 +11309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="44:67">
+    <row r="127" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR127" s="2" t="s">
         <v>37</v>
       </c>
@@ -11369,7 +11377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="44:67">
+    <row r="128" spans="44:67" x14ac:dyDescent="0.2">
       <c r="AR128" s="2" t="s">
         <v>38</v>
       </c>
@@ -11437,7 +11445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:67">
+    <row r="129" spans="1:67" x14ac:dyDescent="0.2">
       <c r="AR129" s="2" t="s">
         <v>39</v>
       </c>
@@ -11505,33 +11513,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:67">
-      <c r="AS130" s="13" t="s">
+    <row r="130" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="AS130" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AT130" s="14"/>
-      <c r="AU130" s="14"/>
-      <c r="AV130" s="14"/>
-      <c r="AW130" s="14"/>
-      <c r="AX130" s="14"/>
-      <c r="AY130" s="14"/>
-      <c r="AZ130" s="14"/>
-      <c r="BA130" s="14"/>
-      <c r="BB130" s="14"/>
-      <c r="BC130" s="14"/>
-      <c r="BD130" s="14"/>
-      <c r="BE130" s="14"/>
-      <c r="BF130" s="14"/>
-      <c r="BG130" s="14"/>
-      <c r="BH130" s="14"/>
-      <c r="BI130" s="14"/>
-      <c r="BJ130" s="14"/>
-      <c r="BK130" s="14"/>
-      <c r="BO130" s="13" t="s">
+      <c r="AT130" s="13"/>
+      <c r="AU130" s="13"/>
+      <c r="AV130" s="13"/>
+      <c r="AW130" s="13"/>
+      <c r="AX130" s="13"/>
+      <c r="AY130" s="13"/>
+      <c r="AZ130" s="13"/>
+      <c r="BA130" s="13"/>
+      <c r="BB130" s="13"/>
+      <c r="BC130" s="13"/>
+      <c r="BD130" s="13"/>
+      <c r="BE130" s="13"/>
+      <c r="BF130" s="13"/>
+      <c r="BG130" s="13"/>
+      <c r="BH130" s="13"/>
+      <c r="BI130" s="13"/>
+      <c r="BJ130" s="13"/>
+      <c r="BK130" s="13"/>
+      <c r="BO130" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:67" ht="184.8">
+    <row r="133" spans="1:67" ht="189" x14ac:dyDescent="0.2">
       <c r="B133" s="3" t="s">
         <v>0</v>
       </c>
@@ -11653,7 +11661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:67">
+    <row r="134" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>68</v>
       </c>
@@ -11778,7 +11786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:67">
+    <row r="135" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>69</v>
       </c>
@@ -11903,7 +11911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:67">
+    <row r="136" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>70</v>
       </c>
@@ -12028,7 +12036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:67">
+    <row r="137" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>71</v>
       </c>
@@ -12153,7 +12161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:67">
+    <row r="138" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>72</v>
       </c>
@@ -12278,7 +12286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:67">
+    <row r="139" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>73</v>
       </c>
@@ -12403,7 +12411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:67">
+    <row r="140" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>74</v>
       </c>
@@ -12528,7 +12536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:67">
+    <row r="141" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>75</v>
       </c>
@@ -12653,7 +12661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:67">
+    <row r="142" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>76</v>
       </c>
@@ -12778,7 +12786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:67">
+    <row r="143" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>77</v>
       </c>
@@ -12903,7 +12911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:67">
+    <row r="144" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>78</v>
       </c>
@@ -13028,7 +13036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:41">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>79</v>
       </c>
@@ -13153,7 +13161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:41">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>80</v>
       </c>
@@ -13278,7 +13286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:41">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>81</v>
       </c>
@@ -13403,7 +13411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:41">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>82</v>
       </c>
@@ -13528,7 +13536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:41">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>83</v>
       </c>
@@ -13653,7 +13661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:41">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>84</v>
       </c>
@@ -13778,7 +13786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:41">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>85</v>
       </c>
@@ -13903,7 +13911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:41">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>86</v>
       </c>
@@ -14028,51 +14036,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:41">
-      <c r="B153" s="13" t="s">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B153" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C153" s="14"/>
-      <c r="D153" s="14"/>
-      <c r="E153" s="14"/>
-      <c r="F153" s="14"/>
-      <c r="G153" s="14"/>
-      <c r="H153" s="14"/>
-      <c r="I153" s="14"/>
-      <c r="J153" s="14"/>
-      <c r="K153" s="14"/>
-      <c r="L153" s="14"/>
-      <c r="M153" s="14"/>
-      <c r="N153" s="14"/>
-      <c r="O153" s="14"/>
-      <c r="P153" s="14"/>
-      <c r="Q153" s="14"/>
-      <c r="R153" s="14"/>
-      <c r="S153" s="14"/>
-      <c r="T153" s="14"/>
-      <c r="U153" s="14"/>
-      <c r="V153" s="14"/>
-      <c r="W153" s="14"/>
-      <c r="X153" s="14"/>
-      <c r="Y153" s="14"/>
-      <c r="Z153" s="14"/>
-      <c r="AA153" s="14"/>
-      <c r="AB153" s="14"/>
-      <c r="AC153" s="14"/>
-      <c r="AD153" s="14"/>
-      <c r="AE153" s="14"/>
-      <c r="AF153" s="14"/>
-      <c r="AG153" s="14"/>
-      <c r="AH153" s="14"/>
-      <c r="AI153" s="14"/>
-      <c r="AJ153" s="14"/>
-      <c r="AK153" s="14"/>
-      <c r="AL153" s="14"/>
-      <c r="AM153" s="14"/>
-      <c r="AN153" s="14"/>
-      <c r="AO153" s="14"/>
-    </row>
-    <row r="156" spans="1:41" ht="184.8">
+      <c r="C153" s="13"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="13"/>
+      <c r="J153" s="13"/>
+      <c r="K153" s="13"/>
+      <c r="L153" s="13"/>
+      <c r="M153" s="13"/>
+      <c r="N153" s="13"/>
+      <c r="O153" s="13"/>
+      <c r="P153" s="13"/>
+      <c r="Q153" s="13"/>
+      <c r="R153" s="13"/>
+      <c r="S153" s="13"/>
+      <c r="T153" s="13"/>
+      <c r="U153" s="13"/>
+      <c r="V153" s="13"/>
+      <c r="W153" s="13"/>
+      <c r="X153" s="13"/>
+      <c r="Y153" s="13"/>
+      <c r="Z153" s="13"/>
+      <c r="AA153" s="13"/>
+      <c r="AB153" s="13"/>
+      <c r="AC153" s="13"/>
+      <c r="AD153" s="13"/>
+      <c r="AE153" s="13"/>
+      <c r="AF153" s="13"/>
+      <c r="AG153" s="13"/>
+      <c r="AH153" s="13"/>
+      <c r="AI153" s="13"/>
+      <c r="AJ153" s="13"/>
+      <c r="AK153" s="13"/>
+      <c r="AL153" s="13"/>
+      <c r="AM153" s="13"/>
+      <c r="AN153" s="13"/>
+      <c r="AO153" s="13"/>
+    </row>
+    <row r="156" spans="1:41" ht="189" x14ac:dyDescent="0.2">
       <c r="B156" s="3" t="s">
         <v>0</v>
       </c>
@@ -14194,7 +14202,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:41">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>40</v>
       </c>
@@ -14319,7 +14327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:41">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>41</v>
       </c>
@@ -14444,7 +14452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:41">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>42</v>
       </c>
@@ -14569,7 +14577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:41">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>43</v>
       </c>
@@ -14694,7 +14702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:41">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>44</v>
       </c>
@@ -14819,7 +14827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:41">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>45</v>
       </c>
@@ -14944,7 +14952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:41">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>46</v>
       </c>
@@ -15069,7 +15077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:41">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>47</v>
       </c>
@@ -15194,7 +15202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:41">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>48</v>
       </c>
@@ -15319,7 +15327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:41">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>49</v>
       </c>
@@ -15444,7 +15452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:41">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>50</v>
       </c>
@@ -15569,7 +15577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:41">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>51</v>
       </c>
@@ -15694,7 +15702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:41">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>52</v>
       </c>
@@ -15819,7 +15827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:41">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>53</v>
       </c>
@@ -15944,7 +15952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:41">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>54</v>
       </c>
@@ -16069,7 +16077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:41">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>55</v>
       </c>
@@ -16194,7 +16202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:41">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>56</v>
       </c>
@@ -16319,7 +16327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:41">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>57</v>
       </c>
@@ -16444,7 +16452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:41">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>58</v>
       </c>
@@ -16569,7 +16577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:41">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>59</v>
       </c>
@@ -16694,7 +16702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:41">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>60</v>
       </c>
@@ -16819,7 +16827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:41">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>61</v>
       </c>
@@ -16944,7 +16952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:41">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>62</v>
       </c>
@@ -17069,7 +17077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:41">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>63</v>
       </c>
@@ -17194,7 +17202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:41">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>64</v>
       </c>
@@ -17319,7 +17327,7 @@
         <v>43.206119998678503</v>
       </c>
     </row>
-    <row r="182" spans="1:41">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>65</v>
       </c>
@@ -17444,7 +17452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:41">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>66</v>
       </c>
@@ -17569,62 +17577,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:41">
-      <c r="B184" s="13" t="s">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B184" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C184" s="14"/>
-      <c r="D184" s="14"/>
-      <c r="E184" s="14"/>
-      <c r="F184" s="14"/>
-      <c r="G184" s="14"/>
-      <c r="H184" s="14"/>
-      <c r="I184" s="14"/>
-      <c r="J184" s="14"/>
-      <c r="K184" s="14"/>
-      <c r="L184" s="14"/>
-      <c r="M184" s="14"/>
-      <c r="N184" s="14"/>
-      <c r="O184" s="14"/>
-      <c r="P184" s="14"/>
-      <c r="Q184" s="14"/>
-      <c r="R184" s="14"/>
-      <c r="S184" s="14"/>
-      <c r="T184" s="14"/>
-      <c r="U184" s="14"/>
-      <c r="V184" s="14"/>
-      <c r="W184" s="14"/>
-      <c r="X184" s="14"/>
-      <c r="Y184" s="14"/>
-      <c r="Z184" s="14"/>
-      <c r="AA184" s="14"/>
-      <c r="AB184" s="14"/>
-      <c r="AC184" s="14"/>
-      <c r="AD184" s="14"/>
-      <c r="AE184" s="14"/>
-      <c r="AF184" s="14"/>
-      <c r="AG184" s="14"/>
-      <c r="AH184" s="14"/>
-      <c r="AI184" s="14"/>
-      <c r="AJ184" s="14"/>
-      <c r="AK184" s="14"/>
-      <c r="AL184" s="14"/>
-      <c r="AM184" s="14"/>
-      <c r="AN184" s="14"/>
-      <c r="AO184" s="14"/>
-    </row>
-    <row r="190" spans="1:41">
-      <c r="B190" s="12" t="s">
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="13"/>
+      <c r="J184" s="13"/>
+      <c r="K184" s="13"/>
+      <c r="L184" s="13"/>
+      <c r="M184" s="13"/>
+      <c r="N184" s="13"/>
+      <c r="O184" s="13"/>
+      <c r="P184" s="13"/>
+      <c r="Q184" s="13"/>
+      <c r="R184" s="13"/>
+      <c r="S184" s="13"/>
+      <c r="T184" s="13"/>
+      <c r="U184" s="13"/>
+      <c r="V184" s="13"/>
+      <c r="W184" s="13"/>
+      <c r="X184" s="13"/>
+      <c r="Y184" s="13"/>
+      <c r="Z184" s="13"/>
+      <c r="AA184" s="13"/>
+      <c r="AB184" s="13"/>
+      <c r="AC184" s="13"/>
+      <c r="AD184" s="13"/>
+      <c r="AE184" s="13"/>
+      <c r="AF184" s="13"/>
+      <c r="AG184" s="13"/>
+      <c r="AH184" s="13"/>
+      <c r="AI184" s="13"/>
+      <c r="AJ184" s="13"/>
+      <c r="AK184" s="13"/>
+      <c r="AL184" s="13"/>
+      <c r="AM184" s="13"/>
+      <c r="AN184" s="13"/>
+      <c r="AO184" s="13"/>
+    </row>
+    <row r="190" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B190" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C190" s="12"/>
-      <c r="D190" s="12"/>
-      <c r="E190" s="12"/>
-      <c r="F190" s="12"/>
-      <c r="G190" s="12"/>
-      <c r="H190" s="12"/>
-    </row>
-    <row r="193" spans="1:6">
+      <c r="C190" s="14"/>
+      <c r="D190" s="14"/>
+      <c r="E190" s="14"/>
+      <c r="F190" s="14"/>
+      <c r="G190" s="14"/>
+      <c r="H190" s="14"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>68</v>
       </c>
@@ -17641,7 +17649,7 @@
         <v>1.6324158541495901E-11</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>69</v>
       </c>
@@ -17658,7 +17666,7 @@
         <v>-3.3648644901857331E-13</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>70</v>
       </c>
@@ -17667,7 +17675,7 @@
         <v>80113.817233021196</v>
       </c>
       <c r="D195" s="10">
-        <f t="shared" ref="D194:D211" si="1">SUM(B136:AO136)</f>
+        <f t="shared" ref="D195:D211" si="1">SUM(B136:AO136)</f>
         <v>16030.243919636299</v>
       </c>
       <c r="F195" s="10">
@@ -17675,7 +17683,7 @@
         <v>64083.573313384899</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>71</v>
       </c>
@@ -17692,7 +17700,7 @@
         <v>5820.7321553383954</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>72</v>
       </c>
@@ -17709,7 +17717,7 @@
         <v>1.20539567973109E-11</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>73</v>
       </c>
@@ -17726,7 +17734,7 @@
         <v>-6.0944432922802798E-10</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>74</v>
       </c>
@@ -17743,7 +17751,7 @@
         <v>4754.0865835986997</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>75</v>
       </c>
@@ -17760,7 +17768,7 @@
         <v>2251368.1944213752</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>76</v>
       </c>
@@ -17783,7 +17791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>77</v>
       </c>
@@ -17800,7 +17808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>78</v>
       </c>
@@ -17817,7 +17825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>79</v>
       </c>
@@ -17834,7 +17842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>80</v>
       </c>
@@ -17851,7 +17859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>81</v>
       </c>
@@ -17868,7 +17876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>82</v>
       </c>
@@ -17885,7 +17893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>83</v>
       </c>
@@ -17902,7 +17910,7 @@
         <v>123739.9739028094</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>84</v>
       </c>
@@ -17919,7 +17927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>85</v>
       </c>
@@ -17936,7 +17944,7 @@
         <v>7801.4912335556583</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>86</v>
       </c>
@@ -17953,7 +17961,7 @@
         <v>-1524.7511711524603</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="16.8">
+    <row r="212" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B212" s="8" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Irreversibilities (have an issue with the named range from ecc xlsx)
</commit_message>
<xml_diff>
--- a/data/ecc_supply_to_mcc.xlsx
+++ b/data/ecc_supply_to_mcc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschu\Documents\github\MaterialExergyPaper2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B1A1B9-0A22-F54B-B3AD-93F4910C1E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC793BC8-7529-463D-8408-2D7EEE444937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38540" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10992" yWindow="192" windowWidth="11928" windowHeight="12516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZAF_2013_X" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="U_EIOU" localSheetId="0">ZAF_2013_X!$AR$1:$BK$41</definedName>
     <definedName name="U_feed" localSheetId="0">ZAF_2013_X!$AR$45:$BK$85</definedName>
     <definedName name="V" localSheetId="0">ZAF_2013_X!$A$133:$AO$152</definedName>
+    <definedName name="X_loss">ZAF_2013_X!$B$193:$F$211</definedName>
     <definedName name="Y" localSheetId="0">ZAF_2013_X!$BN$89:$BO$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -397,7 +398,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -824,38 +825,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F213" sqref="F213"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="28" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="41" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="8.5"/>
+    <col min="42" max="43" width="8.44140625"/>
     <col min="44" max="44" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="65" width="8.5"/>
+    <col min="45" max="65" width="8.44140625"/>
     <col min="66" max="66" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="192" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:85" ht="181.8">
       <c r="B1" s="3" t="s">
         <v>94</v>
       </c>
@@ -974,7 +975,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:85">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:85">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:85">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:85">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:85">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:85">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1742,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:85">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1870,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:85">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:85">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:85">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2254,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:85">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:85">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:85">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:85">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:85">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:85">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:85">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:85">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:85">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -3406,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:85">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -3534,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:85">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -3662,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:85">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:85">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:85">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:85">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -4174,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:85">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -4302,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:85">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:85">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -4558,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:85">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -4686,7 +4687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:85">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -4814,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:85">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -4942,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:85">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -5070,7 +5071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:85">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -5198,7 +5199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:85">
       <c r="A35" s="2" t="s">
         <v>97</v>
       </c>
@@ -5326,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:85">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
@@ -5454,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:85">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -5582,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:85">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:85">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -5838,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:85">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -5966,7 +5967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:85">
       <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
@@ -6094,7 +6095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:85">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -6144,7 +6145,7 @@
       <c r="CF42" s="13"/>
       <c r="CG42" s="13"/>
     </row>
-    <row r="43" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:85">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
@@ -6152,7 +6153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:85">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
@@ -6160,7 +6161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:85" ht="192" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:85" ht="181.8">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
@@ -6225,7 +6226,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:85">
       <c r="B46" s="12" t="s">
         <v>99</v>
       </c>
@@ -6290,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:85">
       <c r="AR47" s="2" t="s">
         <v>1</v>
       </c>
@@ -6352,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:85">
       <c r="AR48" s="2" t="s">
         <v>2</v>
       </c>
@@ -6414,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="49" spans="44:63">
       <c r="AR49" s="2" t="s">
         <v>3</v>
       </c>
@@ -6476,7 +6477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="50" spans="44:63">
       <c r="AR50" s="2" t="s">
         <v>4</v>
       </c>
@@ -6538,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="51" spans="44:63">
       <c r="AR51" s="2" t="s">
         <v>5</v>
       </c>
@@ -6600,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="52" spans="44:63">
       <c r="AR52" s="2" t="s">
         <v>6</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="53" spans="44:63">
       <c r="AR53" s="2" t="s">
         <v>7</v>
       </c>
@@ -6724,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="54" spans="44:63">
       <c r="AR54" s="2" t="s">
         <v>8</v>
       </c>
@@ -6786,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="55" spans="44:63">
       <c r="AR55" s="2" t="s">
         <v>9</v>
       </c>
@@ -6848,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="56" spans="44:63">
       <c r="AR56" s="2" t="s">
         <v>10</v>
       </c>
@@ -6910,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="57" spans="44:63">
       <c r="AR57" s="2" t="s">
         <v>11</v>
       </c>
@@ -6972,7 +6973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="58" spans="44:63">
       <c r="AR58" s="2" t="s">
         <v>12</v>
       </c>
@@ -7034,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="59" spans="44:63">
       <c r="AR59" s="2" t="s">
         <v>13</v>
       </c>
@@ -7096,7 +7097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="60" spans="44:63">
       <c r="AR60" s="2" t="s">
         <v>14</v>
       </c>
@@ -7158,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="61" spans="44:63">
       <c r="AR61" s="2" t="s">
         <v>15</v>
       </c>
@@ -7220,7 +7221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="62" spans="44:63">
       <c r="AR62" s="2" t="s">
         <v>16</v>
       </c>
@@ -7282,7 +7283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="63" spans="44:63">
       <c r="AR63" s="2" t="s">
         <v>17</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="64" spans="44:63">
       <c r="AR64" s="2" t="s">
         <v>18</v>
       </c>
@@ -7406,7 +7407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="65" spans="44:63">
       <c r="AR65" s="2" t="s">
         <v>19</v>
       </c>
@@ -7468,7 +7469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="66" spans="44:63">
       <c r="AR66" s="2" t="s">
         <v>20</v>
       </c>
@@ -7530,7 +7531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="67" spans="44:63">
       <c r="AR67" s="2" t="s">
         <v>21</v>
       </c>
@@ -7592,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="68" spans="44:63">
       <c r="AR68" s="2" t="s">
         <v>22</v>
       </c>
@@ -7654,7 +7655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="69" spans="44:63">
       <c r="AR69" s="2" t="s">
         <v>23</v>
       </c>
@@ -7716,7 +7717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="70" spans="44:63">
       <c r="AR70" s="2" t="s">
         <v>24</v>
       </c>
@@ -7778,7 +7779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="71" spans="44:63">
       <c r="AR71" s="2" t="s">
         <v>25</v>
       </c>
@@ -7840,7 +7841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="72" spans="44:63">
       <c r="AR72" s="2" t="s">
         <v>26</v>
       </c>
@@ -7902,7 +7903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="73" spans="44:63">
       <c r="AR73" s="2" t="s">
         <v>27</v>
       </c>
@@ -7964,7 +7965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="74" spans="44:63">
       <c r="AR74" s="2" t="s">
         <v>28</v>
       </c>
@@ -8026,7 +8027,7 @@
         <v>21683.690906267198</v>
       </c>
     </row>
-    <row r="75" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="75" spans="44:63">
       <c r="AR75" s="2" t="s">
         <v>29</v>
       </c>
@@ -8088,7 +8089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="76" spans="44:63">
       <c r="AR76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8150,7 +8151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="77" spans="44:63">
       <c r="AR77" s="2" t="s">
         <v>31</v>
       </c>
@@ -8212,7 +8213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="78" spans="44:63">
       <c r="AR78" s="2" t="s">
         <v>32</v>
       </c>
@@ -8274,7 +8275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="79" spans="44:63">
       <c r="AR79" s="2" t="s">
         <v>33</v>
       </c>
@@ -8336,7 +8337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="44:63" x14ac:dyDescent="0.2">
+    <row r="80" spans="44:63">
       <c r="AR80" s="2" t="s">
         <v>34</v>
       </c>
@@ -8398,7 +8399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="81" spans="44:67">
       <c r="AR81" s="2" t="s">
         <v>35</v>
       </c>
@@ -8460,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="82" spans="44:67">
       <c r="AR82" s="2" t="s">
         <v>36</v>
       </c>
@@ -8522,7 +8523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="83" spans="44:67">
       <c r="AR83" s="2" t="s">
         <v>37</v>
       </c>
@@ -8584,7 +8585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="84" spans="44:67">
       <c r="AR84" s="2" t="s">
         <v>38</v>
       </c>
@@ -8646,7 +8647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="85" spans="44:67">
       <c r="AR85" s="2" t="s">
         <v>39</v>
       </c>
@@ -8708,7 +8709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="86" spans="44:67">
       <c r="AS86" s="12" t="s">
         <v>93</v>
       </c>
@@ -8731,7 +8732,7 @@
       <c r="BJ86" s="13"/>
       <c r="BK86" s="13"/>
     </row>
-    <row r="89" spans="44:67" ht="192" x14ac:dyDescent="0.2">
+    <row r="89" spans="44:67" ht="181.8">
       <c r="AS89" s="3" t="s">
         <v>68</v>
       </c>
@@ -8793,7 +8794,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="90" spans="44:67">
       <c r="AR90" s="2" t="s">
         <v>0</v>
       </c>
@@ -8861,7 +8862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="91" spans="44:67">
       <c r="AR91" s="2" t="s">
         <v>1</v>
       </c>
@@ -8929,7 +8930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="92" spans="44:67">
       <c r="AR92" s="2" t="s">
         <v>2</v>
       </c>
@@ -8997,7 +8998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="93" spans="44:67">
       <c r="AR93" s="2" t="s">
         <v>3</v>
       </c>
@@ -9065,7 +9066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="94" spans="44:67">
       <c r="AR94" s="2" t="s">
         <v>4</v>
       </c>
@@ -9133,7 +9134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="95" spans="44:67">
       <c r="AR95" s="2" t="s">
         <v>5</v>
       </c>
@@ -9201,7 +9202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="96" spans="44:67">
       <c r="AR96" s="2" t="s">
         <v>6</v>
       </c>
@@ -9269,7 +9270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="97" spans="44:67">
       <c r="AR97" s="2" t="s">
         <v>7</v>
       </c>
@@ -9337,7 +9338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="98" spans="44:67">
       <c r="AR98" s="2" t="s">
         <v>8</v>
       </c>
@@ -9405,7 +9406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="99" spans="44:67">
       <c r="AR99" s="2" t="s">
         <v>9</v>
       </c>
@@ -9473,7 +9474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="100" spans="44:67">
       <c r="AR100" s="2" t="s">
         <v>10</v>
       </c>
@@ -9541,7 +9542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="101" spans="44:67">
       <c r="AR101" s="2" t="s">
         <v>11</v>
       </c>
@@ -9609,7 +9610,7 @@
         <v>1058348.7350491199</v>
       </c>
     </row>
-    <row r="102" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="102" spans="44:67">
       <c r="AR102" s="2" t="s">
         <v>12</v>
       </c>
@@ -9677,7 +9678,7 @@
         <v>29112.263489807599</v>
       </c>
     </row>
-    <row r="103" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="103" spans="44:67">
       <c r="AR103" s="2" t="s">
         <v>13</v>
       </c>
@@ -9745,7 +9746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="104" spans="44:67">
       <c r="AR104" s="2" t="s">
         <v>14</v>
       </c>
@@ -9813,7 +9814,7 @@
         <v>117713.246391553</v>
       </c>
     </row>
-    <row r="105" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="105" spans="44:67">
       <c r="AR105" s="2" t="s">
         <v>15</v>
       </c>
@@ -9881,7 +9882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="106" spans="44:67">
       <c r="AR106" s="2" t="s">
         <v>16</v>
       </c>
@@ -9949,7 +9950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="107" spans="44:67">
       <c r="AR107" s="2" t="s">
         <v>17</v>
       </c>
@@ -10017,7 +10018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="108" spans="44:67">
       <c r="AR108" s="2" t="s">
         <v>18</v>
       </c>
@@ -10085,7 +10086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="109" spans="44:67">
       <c r="AR109" s="2" t="s">
         <v>19</v>
       </c>
@@ -10153,7 +10154,7 @@
         <v>24.076233417548501</v>
       </c>
     </row>
-    <row r="110" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="110" spans="44:67">
       <c r="AR110" s="2" t="s">
         <v>20</v>
       </c>
@@ -10221,7 +10222,7 @@
         <v>14864300.6683855</v>
       </c>
     </row>
-    <row r="111" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="111" spans="44:67">
       <c r="AR111" s="2" t="s">
         <v>21</v>
       </c>
@@ -10289,7 +10290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="112" spans="44:67">
       <c r="AR112" s="2" t="s">
         <v>22</v>
       </c>
@@ -10357,7 +10358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="113" spans="44:67">
       <c r="AR113" s="2" t="s">
         <v>23</v>
       </c>
@@ -10425,7 +10426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="114" spans="44:67">
       <c r="AR114" s="2" t="s">
         <v>24</v>
       </c>
@@ -10493,7 +10494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="115" spans="44:67">
       <c r="AR115" s="2" t="s">
         <v>25</v>
       </c>
@@ -10561,7 +10562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="116" spans="44:67">
       <c r="AR116" s="2" t="s">
         <v>26</v>
       </c>
@@ -10629,7 +10630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="117" spans="44:67">
       <c r="AR117" s="2" t="s">
         <v>27</v>
       </c>
@@ -10697,7 +10698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="118" spans="44:67">
       <c r="AR118" s="2" t="s">
         <v>28</v>
       </c>
@@ -10765,7 +10766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="119" spans="44:67">
       <c r="AR119" s="2" t="s">
         <v>29</v>
       </c>
@@ -10833,7 +10834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="120" spans="44:67">
       <c r="AR120" s="2" t="s">
         <v>30</v>
       </c>
@@ -10901,7 +10902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="121" spans="44:67">
       <c r="AR121" s="2" t="s">
         <v>31</v>
       </c>
@@ -10969,7 +10970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="122" spans="44:67">
       <c r="AR122" s="2" t="s">
         <v>32</v>
       </c>
@@ -11037,7 +11038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="123" spans="44:67">
       <c r="AR123" s="2" t="s">
         <v>33</v>
       </c>
@@ -11105,7 +11106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="124" spans="44:67">
       <c r="AR124" s="2" t="s">
         <v>34</v>
       </c>
@@ -11173,7 +11174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="125" spans="44:67">
       <c r="AR125" s="2" t="s">
         <v>35</v>
       </c>
@@ -11241,7 +11242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="126" spans="44:67">
       <c r="AR126" s="2" t="s">
         <v>36</v>
       </c>
@@ -11309,7 +11310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="127" spans="44:67">
       <c r="AR127" s="2" t="s">
         <v>37</v>
       </c>
@@ -11377,7 +11378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="44:67" x14ac:dyDescent="0.2">
+    <row r="128" spans="44:67">
       <c r="AR128" s="2" t="s">
         <v>38</v>
       </c>
@@ -11445,7 +11446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:67">
       <c r="AR129" s="2" t="s">
         <v>39</v>
       </c>
@@ -11513,7 +11514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:67">
       <c r="AS130" s="12" t="s">
         <v>87</v>
       </c>
@@ -11539,7 +11540,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:67" ht="189" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:67" ht="184.8">
       <c r="B133" s="3" t="s">
         <v>0</v>
       </c>
@@ -11661,7 +11662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:67">
       <c r="A134" s="2" t="s">
         <v>68</v>
       </c>
@@ -11786,7 +11787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:67">
       <c r="A135" s="2" t="s">
         <v>69</v>
       </c>
@@ -11911,7 +11912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:67">
       <c r="A136" s="2" t="s">
         <v>70</v>
       </c>
@@ -12036,7 +12037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:67">
       <c r="A137" s="2" t="s">
         <v>71</v>
       </c>
@@ -12161,7 +12162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:67">
       <c r="A138" s="2" t="s">
         <v>72</v>
       </c>
@@ -12286,7 +12287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:67">
       <c r="A139" s="2" t="s">
         <v>73</v>
       </c>
@@ -12411,7 +12412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:67">
       <c r="A140" s="2" t="s">
         <v>74</v>
       </c>
@@ -12536,7 +12537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:67">
       <c r="A141" s="2" t="s">
         <v>75</v>
       </c>
@@ -12661,7 +12662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:67">
       <c r="A142" s="2" t="s">
         <v>76</v>
       </c>
@@ -12786,7 +12787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:67">
       <c r="A143" s="2" t="s">
         <v>77</v>
       </c>
@@ -12911,7 +12912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:67">
       <c r="A144" s="2" t="s">
         <v>78</v>
       </c>
@@ -13036,7 +13037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:41">
       <c r="A145" s="2" t="s">
         <v>79</v>
       </c>
@@ -13161,7 +13162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:41">
       <c r="A146" s="2" t="s">
         <v>80</v>
       </c>
@@ -13286,7 +13287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:41">
       <c r="A147" s="2" t="s">
         <v>81</v>
       </c>
@@ -13411,7 +13412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:41">
       <c r="A148" s="2" t="s">
         <v>82</v>
       </c>
@@ -13536,7 +13537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:41">
       <c r="A149" s="2" t="s">
         <v>83</v>
       </c>
@@ -13661,7 +13662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:41">
       <c r="A150" s="2" t="s">
         <v>84</v>
       </c>
@@ -13786,7 +13787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:41">
       <c r="A151" s="2" t="s">
         <v>85</v>
       </c>
@@ -13911,7 +13912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:41">
       <c r="A152" s="2" t="s">
         <v>86</v>
       </c>
@@ -14036,7 +14037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:41">
       <c r="B153" s="12" t="s">
         <v>88</v>
       </c>
@@ -14080,7 +14081,7 @@
       <c r="AN153" s="13"/>
       <c r="AO153" s="13"/>
     </row>
-    <row r="156" spans="1:41" ht="189" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:41" ht="184.8">
       <c r="B156" s="3" t="s">
         <v>0</v>
       </c>
@@ -14202,7 +14203,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:41">
       <c r="A157" s="2" t="s">
         <v>40</v>
       </c>
@@ -14327,7 +14328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:41">
       <c r="A158" s="2" t="s">
         <v>41</v>
       </c>
@@ -14452,7 +14453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:41">
       <c r="A159" s="2" t="s">
         <v>42</v>
       </c>
@@ -14577,7 +14578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:41">
       <c r="A160" s="2" t="s">
         <v>43</v>
       </c>
@@ -14702,7 +14703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:41">
       <c r="A161" s="2" t="s">
         <v>44</v>
       </c>
@@ -14827,7 +14828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:41">
       <c r="A162" s="2" t="s">
         <v>45</v>
       </c>
@@ -14952,7 +14953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:41">
       <c r="A163" s="2" t="s">
         <v>46</v>
       </c>
@@ -15077,7 +15078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:41">
       <c r="A164" s="2" t="s">
         <v>47</v>
       </c>
@@ -15202,7 +15203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:41">
       <c r="A165" s="2" t="s">
         <v>48</v>
       </c>
@@ -15327,7 +15328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:41">
       <c r="A166" s="2" t="s">
         <v>49</v>
       </c>
@@ -15452,7 +15453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:41">
       <c r="A167" s="2" t="s">
         <v>50</v>
       </c>
@@ -15577,7 +15578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:41">
       <c r="A168" s="2" t="s">
         <v>51</v>
       </c>
@@ -15702,7 +15703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:41">
       <c r="A169" s="2" t="s">
         <v>52</v>
       </c>
@@ -15827,7 +15828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:41">
       <c r="A170" s="2" t="s">
         <v>53</v>
       </c>
@@ -15952,7 +15953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:41">
       <c r="A171" s="2" t="s">
         <v>54</v>
       </c>
@@ -16077,7 +16078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:41">
       <c r="A172" s="2" t="s">
         <v>55</v>
       </c>
@@ -16202,7 +16203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:41">
       <c r="A173" s="2" t="s">
         <v>56</v>
       </c>
@@ -16327,7 +16328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:41">
       <c r="A174" s="2" t="s">
         <v>57</v>
       </c>
@@ -16452,7 +16453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:41">
       <c r="A175" s="2" t="s">
         <v>58</v>
       </c>
@@ -16577,7 +16578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:41">
       <c r="A176" s="2" t="s">
         <v>59</v>
       </c>
@@ -16702,7 +16703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:41">
       <c r="A177" s="2" t="s">
         <v>60</v>
       </c>
@@ -16827,7 +16828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:41">
       <c r="A178" s="2" t="s">
         <v>61</v>
       </c>
@@ -16952,7 +16953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:41">
       <c r="A179" s="2" t="s">
         <v>62</v>
       </c>
@@ -17077,7 +17078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:41">
       <c r="A180" s="2" t="s">
         <v>63</v>
       </c>
@@ -17202,7 +17203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:41">
       <c r="A181" s="2" t="s">
         <v>64</v>
       </c>
@@ -17327,7 +17328,7 @@
         <v>43.206119998678503</v>
       </c>
     </row>
-    <row r="182" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:41">
       <c r="A182" s="2" t="s">
         <v>65</v>
       </c>
@@ -17452,7 +17453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:41">
       <c r="A183" s="2" t="s">
         <v>66</v>
       </c>
@@ -17577,7 +17578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:41">
       <c r="B184" s="12" t="s">
         <v>67</v>
       </c>
@@ -17621,7 +17622,7 @@
       <c r="AN184" s="13"/>
       <c r="AO184" s="13"/>
     </row>
-    <row r="190" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:41">
       <c r="B190" s="14" t="s">
         <v>102</v>
       </c>
@@ -17632,7 +17633,7 @@
       <c r="G190" s="14"/>
       <c r="H190" s="14"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6">
       <c r="A193" s="2" t="s">
         <v>68</v>
       </c>
@@ -17649,7 +17650,7 @@
         <v>1.6324158541495901E-11</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6">
       <c r="A194" s="2" t="s">
         <v>69</v>
       </c>
@@ -17666,7 +17667,7 @@
         <v>-3.3648644901857331E-13</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6">
       <c r="A195" s="2" t="s">
         <v>70</v>
       </c>
@@ -17683,7 +17684,7 @@
         <v>64083.573313384899</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6">
       <c r="A196" s="2" t="s">
         <v>71</v>
       </c>
@@ -17700,7 +17701,7 @@
         <v>5820.7321553383954</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
         <v>72</v>
       </c>
@@ -17717,7 +17718,7 @@
         <v>1.20539567973109E-11</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6">
       <c r="A198" s="2" t="s">
         <v>73</v>
       </c>
@@ -17734,7 +17735,7 @@
         <v>-6.0944432922802798E-10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6">
       <c r="A199" s="2" t="s">
         <v>74</v>
       </c>
@@ -17751,7 +17752,7 @@
         <v>4754.0865835986997</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6">
       <c r="A200" s="2" t="s">
         <v>75</v>
       </c>
@@ -17768,7 +17769,7 @@
         <v>2251368.1944213752</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6">
       <c r="A201" s="2" t="s">
         <v>76</v>
       </c>
@@ -17791,7 +17792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6">
       <c r="A202" s="2" t="s">
         <v>77</v>
       </c>
@@ -17808,7 +17809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6">
       <c r="A203" s="2" t="s">
         <v>78</v>
       </c>
@@ -17825,7 +17826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6">
       <c r="A204" s="2" t="s">
         <v>79</v>
       </c>
@@ -17842,7 +17843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6">
       <c r="A205" s="2" t="s">
         <v>80</v>
       </c>
@@ -17859,7 +17860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6">
       <c r="A206" s="2" t="s">
         <v>81</v>
       </c>
@@ -17876,7 +17877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6">
       <c r="A207" s="2" t="s">
         <v>82</v>
       </c>
@@ -17893,7 +17894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6">
       <c r="A208" s="2" t="s">
         <v>83</v>
       </c>
@@ -17910,7 +17911,7 @@
         <v>123739.9739028094</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6">
       <c r="A209" s="2" t="s">
         <v>84</v>
       </c>
@@ -17927,7 +17928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6">
       <c r="A210" s="2" t="s">
         <v>85</v>
       </c>
@@ -17944,7 +17945,7 @@
         <v>7801.4912335556583</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6">
       <c r="A211" s="2" t="s">
         <v>86</v>
       </c>
@@ -17961,7 +17962,7 @@
         <v>-1524.7511711524603</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" ht="16.8">
       <c r="B212" s="8" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Irreversibility and conversion chain description tables
</commit_message>
<xml_diff>
--- a/data/ecc_supply_to_mcc.xlsx
+++ b/data/ecc_supply_to_mcc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschu\Documents\github\MaterialExergyPaper2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC793BC8-7529-463D-8408-2D7EEE444937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240CF096-E5D3-4EFF-8ECC-440ACD94FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10992" yWindow="192" windowWidth="11928" windowHeight="12516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="12" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZAF_2013_X" sheetId="1" r:id="rId1"/>
@@ -382,9 +382,6 @@
     <t>Vi</t>
   </si>
   <si>
-    <t>Energy balance across industries</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>X_loss</t>
+  </si>
+  <si>
+    <t>Exergy balance across industries</t>
   </si>
 </sst>
 </file>
@@ -826,7 +826,7 @@
   <dimension ref="A1:CG212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A188" zoomScale="98" workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+      <selection activeCell="I202" sqref="I202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -17624,7 +17624,7 @@
     </row>
     <row r="190" spans="1:41">
       <c r="B190" s="14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C190" s="14"/>
       <c r="D190" s="14"/>
@@ -17778,14 +17778,14 @@
         <v>4830.4442158522497</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D201" s="10">
         <f t="shared" si="1"/>
         <v>4830.4442158522497</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F201" s="10">
         <f t="shared" si="0"/>
@@ -17971,7 +17971,7 @@
         <v>101</v>
       </c>
       <c r="F212" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>